<commit_message>
dat final push babbyyyy :OOOO
</commit_message>
<xml_diff>
--- a/Experimental Data/Data Graphs.xlsx
+++ b/Experimental Data/Data Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wsolow\Desktop\CS446\CS446\Experimental Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA09091E-7682-4E9A-9526-E0E390DA9D31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A922436-FF9F-4D74-BD1E-98F8EC202A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E8585C4-C860-42BC-83FC-8C17E514B67F}"/>
+    <workbookView xWindow="10455" yWindow="180" windowWidth="17010" windowHeight="14715" xr2:uid="{0E8585C4-C860-42BC-83FC-8C17E514B67F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
   <si>
     <t xml:space="preserve">Walkers: </t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>sim 10</t>
+  </si>
+  <si>
+    <t> 9998.92473440135</t>
   </si>
 </sst>
 </file>
@@ -5530,8 +5533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17403C00-ED43-4CA2-8BB5-D37A334092CE}">
   <dimension ref="A1:T139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q120" sqref="Q120:S120"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P111" sqref="P111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8070,7 +8073,7 @@
         <v>10000</v>
       </c>
       <c r="P101">
-        <f t="shared" ref="P100:P101" si="5">AVERAGE(B133:K133)</f>
+        <f t="shared" ref="P101" si="5">AVERAGE(B133:K133)</f>
         <v>0.18646843099999999</v>
       </c>
       <c r="Q101">
@@ -8242,9 +8245,9 @@
       <c r="N105">
         <v>10000</v>
       </c>
-      <c r="P105" t="e">
+      <c r="P105">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>0.18647248653671319</v>
       </c>
       <c r="Q105">
         <f t="shared" si="7"/>
@@ -8660,9 +8663,9 @@
       <c r="N116">
         <v>10000</v>
       </c>
-      <c r="P116" t="e">
+      <c r="P116">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>1.5521926008014625E-4</v>
       </c>
       <c r="Q116">
         <f t="shared" si="15"/>
@@ -8780,6 +8783,10 @@
       <c r="K120">
         <v>0.18573445</v>
       </c>
+      <c r="P120">
+        <f>AVERAGE(B135:K135)/10000</f>
+        <v>0.99988682579920152</v>
+      </c>
       <c r="Q120">
         <f>AVERAGE(B124:K124)/10000</f>
         <v>0.99739460000000002</v>
@@ -9125,6 +9132,36 @@
       <c r="A135" t="s">
         <v>25</v>
       </c>
+      <c r="B135" s="2">
+        <v>9998.9351537999992</v>
+      </c>
+      <c r="C135" s="2">
+        <v>9998.94281618887</v>
+      </c>
+      <c r="D135" s="2">
+        <v>9998.98082209106</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F135" s="2">
+        <v>9998.9061298482193</v>
+      </c>
+      <c r="G135" s="2">
+        <v>9998.9699999999993</v>
+      </c>
+      <c r="H135" s="2">
+        <v>9998.9279999999999</v>
+      </c>
+      <c r="I135" s="2">
+        <v>9998.9226999999992</v>
+      </c>
+      <c r="J135" s="2">
+        <v>9998.9297999999999</v>
+      </c>
+      <c r="K135" s="2">
+        <v>9998.2988999999998</v>
+      </c>
     </row>
     <row r="136" spans="1:11">
       <c r="B136" t="s">
@@ -9204,6 +9241,36 @@
     <row r="139" spans="1:11">
       <c r="A139">
         <v>10000</v>
+      </c>
+      <c r="B139" s="2">
+        <v>0.18623481</v>
+      </c>
+      <c r="C139" s="2">
+        <v>0.18653843065461301</v>
+      </c>
+      <c r="D139" s="2">
+        <v>0.18657723046890801</v>
+      </c>
+      <c r="E139" s="2">
+        <v>0.18672378837418099</v>
+      </c>
+      <c r="F139" s="2">
+        <v>0.18664059282942999</v>
+      </c>
+      <c r="G139" s="2">
+        <v>0.18646527809999999</v>
+      </c>
+      <c r="H139" s="2">
+        <v>0.18630113800000001</v>
+      </c>
+      <c r="I139" s="2">
+        <v>0.18649255470000001</v>
+      </c>
+      <c r="J139" s="2">
+        <v>0.18632554524</v>
+      </c>
+      <c r="K139" s="2">
+        <v>0.186425497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>